<commit_message>
Fixed influienza model. Added t100 market from year 2000. Will be able to compare with results from Grais et al.
</commit_message>
<xml_diff>
--- a/airport/data/dummy_matrix.xlsx
+++ b/airport/data/dummy_matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikaelrs\Skole\Master\Repositories\flutrack_backend\prediction\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikaelrs\Skole\Master\Repositories\flutrack_backend\airport\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AW67" sqref="AW67"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AN42" sqref="AN42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="K3">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="L3">
         <v>10</v>
@@ -2123,7 +2123,7 @@
         <v>69</v>
       </c>
       <c r="C11">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>4</v>

</xml_diff>